<commit_message>
Ajout du concept dans la documentation
</commit_message>
<xml_diff>
--- a/Documentation/2023.05.04_Nonnenmacher_Enzo_Journal de travail.xlsx
+++ b/Documentation/2023.05.04_Nonnenmacher_Enzo_Journal de travail.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Jour</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>Rédaction de la partie "Analyse du logiciel"</t>
+  </si>
+  <si>
+    <t>Analyse des avantages et inconvénients d'utiliser GLPI</t>
+  </si>
+  <si>
+    <t>Rédaction du concept du projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réflexion sur la stratégie de test </t>
+  </si>
+  <si>
+    <t>Rédaction de la planification du projet</t>
   </si>
 </sst>
 </file>
@@ -180,7 +192,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[hh]/mm&quot; h&quot;;@"/>
     </dxf>
@@ -250,13 +265,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F10" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:F10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F14" totalsRowShown="0" headerRowDxfId="12">
+  <autoFilter ref="A1:F14"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Jour" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="2" name="Semaine" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="3" name="Temps [h]" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="4" name="Type" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="1" name="Jour" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="2" name="Semaine" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" name="Temps [h]" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="4" name="Type" dataDxfId="5" totalsRowDxfId="4"/>
     <tableColumn id="5" name="Description"/>
     <tableColumn id="6" name="Commentaire/Remarque"/>
   </tableColumns>
@@ -265,13 +280,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B3" totalsRowCount="1">
-  <autoFilter ref="A1:B2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B4" totalsRowCount="1">
+  <autoFilter ref="A1:B3">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="2" totalsRowDxfId="1"/>
-    <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" totalsRowDxfId="0">
-      <calculatedColumnFormula>SUM(Tableau1[Temps '[h']])</calculatedColumnFormula>
-      <totalsRowFormula>SUM(B2:B2)</totalsRowFormula>
+    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" dataDxfId="0" totalsRowDxfId="1">
+      <calculatedColumnFormula>SUM(Journal!C2:C7)</calculatedColumnFormula>
+      <totalsRowFormula>SUM(B2:B3)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -541,7 +559,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
@@ -726,10 +744,95 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="8"/>
+      <c r="A10" s="7">
+        <v>45050</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>45050</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>45050</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>45050</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>45050</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -742,10 +845,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,22 +870,34 @@
         <v>45048</v>
       </c>
       <c r="B2" s="5">
-        <f>SUM(Tableau1[Temps '[h']])</f>
-        <v>0.27083333333333331</v>
+        <f>SUM(Journal!C2:C7)</f>
+        <v>0.20833333333333331</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6">
+        <v>45050</v>
+      </c>
+      <c r="B3" s="5">
+        <f>SUM(Journal!C8:C14)</f>
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="12">
-        <f>SUM(B2:B2)</f>
-        <v>0.27083333333333331</v>
+      <c r="B4" s="12">
+        <f>SUM(B2:B3)</f>
+        <v>0.41666666666666663</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2" formulaRange="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>